<commit_message>
Add maintenance logs list and detail views, add new fields into maintenance logs, add new field into refrigerators, clean up
</commit_message>
<xml_diff>
--- a/app/config/tables/maintenance_logs/forms/maintenance_logs/maintenance_logs.xlsx
+++ b/app/config/tables/maintenance_logs/forms/maintenance_logs/maintenance_logs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="2500" yWindow="0" windowWidth="33320" windowHeight="19560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="115">
   <si>
     <t>clause</t>
   </si>
@@ -244,15 +244,9 @@
     <t>detailViewFileName</t>
   </si>
   <si>
-    <t>config/assets/aa_m_logs_detail.html</t>
-  </si>
-  <si>
     <t>listViewFileName</t>
   </si>
   <si>
-    <t>config/assets/aa_m_logs_list.html</t>
-  </si>
-  <si>
     <t>security</t>
   </si>
   <si>
@@ -290,6 +284,93 @@
   </si>
   <si>
     <t>maintenance_logs</t>
+  </si>
+  <si>
+    <t>config/tables/maintenance_logs/html/maintenance_logs_detail.html</t>
+  </si>
+  <si>
+    <t>config/tables/maintenance_logs/html/maintenance_logs_list.html</t>
+  </si>
+  <si>
+    <t>type_of_maintenance</t>
+  </si>
+  <si>
+    <t>Type of Maintenance Performed</t>
+  </si>
+  <si>
+    <t>Tipo de mantenimiento realizado</t>
+  </si>
+  <si>
+    <t>select_one</t>
+  </si>
+  <si>
+    <t>maint_types</t>
+  </si>
+  <si>
+    <t>Repair</t>
+  </si>
+  <si>
+    <t>Preventative</t>
+  </si>
+  <si>
+    <t>Inspection</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>repair</t>
+  </si>
+  <si>
+    <t>retrofit</t>
+  </si>
+  <si>
+    <t>preventative</t>
+  </si>
+  <si>
+    <t>inspection</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Reparar</t>
+  </si>
+  <si>
+    <t>Preventivo</t>
+  </si>
+  <si>
+    <t>Inspección</t>
+  </si>
+  <si>
+    <t>Otro</t>
+  </si>
+  <si>
+    <t>Upgrade</t>
+  </si>
+  <si>
+    <t>Mejorar</t>
+  </si>
+  <si>
+    <t>spare_parts</t>
+  </si>
+  <si>
+    <t>Enter spare parts</t>
+  </si>
+  <si>
+    <t>Entrar piezas de repuesto</t>
+  </si>
+  <si>
+    <t>Haga una lista de repuestos</t>
+  </si>
+  <si>
+    <t>Make a list of spare parts</t>
+  </si>
+  <si>
+    <t>Select type of maintenance</t>
+  </si>
+  <si>
+    <t>Seleccione el tipo de mantenimiento</t>
   </si>
 </sst>
 </file>
@@ -364,7 +445,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -383,6 +464,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -786,10 +870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" activeCellId="1" sqref="B5 B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -799,8 +883,10 @@
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" customWidth="1"/>
     <col min="5" max="5" width="20.6640625" customWidth="1"/>
-    <col min="6" max="8" width="24.6640625" customWidth="1"/>
-    <col min="9" max="9" width="21.1640625" customWidth="1"/>
+    <col min="6" max="6" width="32.83203125" customWidth="1"/>
+    <col min="7" max="7" width="32.33203125" customWidth="1"/>
+    <col min="8" max="8" width="24.6640625" customWidth="1"/>
+    <col min="9" max="9" width="39.5" customWidth="1"/>
     <col min="10" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -944,7 +1030,50 @@
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" t="s">
+      <c r="C8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8" t="s">
+        <v>89</v>
+      </c>
+      <c r="G8" t="s">
+        <v>90</v>
+      </c>
+      <c r="H8" t="s">
+        <v>113</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="C9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F9" t="s">
+        <v>109</v>
+      </c>
+      <c r="G9" t="s">
+        <v>110</v>
+      </c>
+      <c r="H9" t="s">
+        <v>112</v>
+      </c>
+      <c r="I9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
         <v>30</v>
       </c>
     </row>
@@ -961,21 +1090,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C2"/>
+  <dimension ref="A2:D7"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C4" activeCellId="1" sqref="B5 C4"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="23.1640625" customWidth="1"/>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" customWidth="1"/>
-    <col min="4" max="1025" width="8.5" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="5" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="20" customHeight="1">
+    <row r="2" spans="1:4" ht="20" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
@@ -984,6 +1114,79 @@
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1085,7 +1288,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1124,7 +1327,7 @@
         <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1132,7 +1335,7 @@
         <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1200,12 +1403,14 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" activeCellId="1" sqref="B5 A7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="4" width="8.5" customWidth="1"/>
+    <col min="1" max="2" width="8.5" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" customWidth="1"/>
     <col min="5" max="5" width="17.5" customWidth="1"/>
     <col min="6" max="1025" width="8.5" customWidth="1"/>
   </cols>
@@ -1258,7 +1463,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1269,13 +1474,13 @@
         <v>68</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1283,16 +1488,16 @@
         <v>67</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="E5" s="8" t="s">
         <v>76</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1300,50 +1505,50 @@
         <v>67</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change CSVs to reflect new columns
</commit_message>
<xml_diff>
--- a/app/config/tables/maintenance_logs/forms/maintenance_logs/maintenance_logs.xlsx
+++ b/app/config/tables/maintenance_logs/forms/maintenance_logs/maintenance_logs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2500" yWindow="0" windowWidth="33320" windowHeight="19560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -322,9 +322,6 @@
     <t>repair</t>
   </si>
   <si>
-    <t>retrofit</t>
-  </si>
-  <si>
     <t>preventative</t>
   </si>
   <si>
@@ -371,6 +368,9 @@
   </si>
   <si>
     <t>Seleccione el tipo de mantenimiento</t>
+  </si>
+  <si>
+    <t>upgrade</t>
   </si>
 </sst>
 </file>
@@ -872,7 +872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -1046,10 +1046,10 @@
         <v>90</v>
       </c>
       <c r="H8" t="s">
+        <v>112</v>
+      </c>
+      <c r="I8" s="9" t="s">
         <v>113</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1057,19 +1057,19 @@
         <v>12</v>
       </c>
       <c r="E9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F9" t="s">
         <v>108</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>109</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
+        <v>111</v>
+      </c>
+      <c r="I9" t="s">
         <v>110</v>
-      </c>
-      <c r="H9" t="s">
-        <v>112</v>
-      </c>
-      <c r="I9" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1092,8 +1092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D7"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1130,7 +1130,7 @@
         <v>93</v>
       </c>
       <c r="D3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1138,13 +1138,13 @@
         <v>92</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="C4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" t="s">
         <v>106</v>
-      </c>
-      <c r="D4" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1152,13 +1152,13 @@
         <v>92</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C5" t="s">
         <v>94</v>
       </c>
       <c r="D5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1166,13 +1166,13 @@
         <v>92</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6" t="s">
         <v>95</v>
       </c>
       <c r="D6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1180,13 +1180,13 @@
         <v>92</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C7" t="s">
         <v>96</v>
       </c>
       <c r="D7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix service query, add in refrigerator status form, fix formatting dates in list view
</commit_message>
<xml_diff>
--- a/app/config/tables/maintenance_logs/forms/maintenance_logs/maintenance_logs.xlsx
+++ b/app/config/tables/maintenance_logs/forms/maintenance_logs/maintenance_logs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2920" yWindow="1300" windowWidth="28360" windowHeight="19560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="176">
   <si>
     <t>clause</t>
   </si>
@@ -352,12 +352,6 @@
     <t>spare_parts</t>
   </si>
   <si>
-    <t>Enter spare parts</t>
-  </si>
-  <si>
-    <t>Entrar piezas de repuesto</t>
-  </si>
-  <si>
     <t>Haga una lista de repuestos</t>
   </si>
   <si>
@@ -371,13 +365,205 @@
   </si>
   <si>
     <t>upgrade</t>
+  </si>
+  <si>
+    <t>select_multiple</t>
+  </si>
+  <si>
+    <t>addtl_spare_parts</t>
+  </si>
+  <si>
+    <t>Spare Parts</t>
+  </si>
+  <si>
+    <t>Enter additional spare parts</t>
+  </si>
+  <si>
+    <t>Entrar adicional piezas de repuesto</t>
+  </si>
+  <si>
+    <t>Piezas de Repuesto</t>
+  </si>
+  <si>
+    <t>Select spare parts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Seleccione piezas de repuestos</t>
+  </si>
+  <si>
+    <t>common_spare_parts</t>
+  </si>
+  <si>
+    <t>condenser_fan</t>
+  </si>
+  <si>
+    <t>electric_compressor</t>
+  </si>
+  <si>
+    <t>thermocouple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">charging_cylinder </t>
+  </si>
+  <si>
+    <t>thermometer</t>
+  </si>
+  <si>
+    <t>solar_compressor</t>
+  </si>
+  <si>
+    <t>rotary_fan</t>
+  </si>
+  <si>
+    <t>leak_detector</t>
+  </si>
+  <si>
+    <t>gas_regulator</t>
+  </si>
+  <si>
+    <t>hose</t>
+  </si>
+  <si>
+    <t>fridge_tag</t>
+  </si>
+  <si>
+    <t>refrigerant</t>
+  </si>
+  <si>
+    <t>thermostat</t>
+  </si>
+  <si>
+    <t>relay</t>
+  </si>
+  <si>
+    <t>burner</t>
+  </si>
+  <si>
+    <t>fuse</t>
+  </si>
+  <si>
+    <t>voltage_regulator</t>
+  </si>
+  <si>
+    <t>door_gasket</t>
+  </si>
+  <si>
+    <t>Condenser Fan</t>
+  </si>
+  <si>
+    <t>Thermostat</t>
+  </si>
+  <si>
+    <t>Relay</t>
+  </si>
+  <si>
+    <t>Refrigerant</t>
+  </si>
+  <si>
+    <t>Electric Compressor</t>
+  </si>
+  <si>
+    <t>Thermocouple</t>
+  </si>
+  <si>
+    <t>Charging Cylinder</t>
+  </si>
+  <si>
+    <t>Thermometer</t>
+  </si>
+  <si>
+    <t>Solar Compressor</t>
+  </si>
+  <si>
+    <t>Rotary Fan</t>
+  </si>
+  <si>
+    <t>Leak Detector</t>
+  </si>
+  <si>
+    <t>Gas Regulator</t>
+  </si>
+  <si>
+    <t>Hose</t>
+  </si>
+  <si>
+    <t>Fridge Tag</t>
+  </si>
+  <si>
+    <t>Burner</t>
+  </si>
+  <si>
+    <t>Fuse</t>
+  </si>
+  <si>
+    <t>Door Gasket</t>
+  </si>
+  <si>
+    <t>Voltage Regulator</t>
+  </si>
+  <si>
+    <t>Quemador</t>
+  </si>
+  <si>
+    <t>Cilindro de carga</t>
+  </si>
+  <si>
+    <t>Ventilador Condensador</t>
+  </si>
+  <si>
+    <t>La Junta de la Puerta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Compresor Eléctrico</t>
+  </si>
+  <si>
+    <t>Etiqueta Frigorífico</t>
+  </si>
+  <si>
+    <t>Fusible</t>
+  </si>
+  <si>
+    <t>Regulador de Gas</t>
+  </si>
+  <si>
+    <t>Manguera</t>
+  </si>
+  <si>
+    <t>Detector de Fugas</t>
+  </si>
+  <si>
+    <t>Relé</t>
+  </si>
+  <si>
+    <t>Refrigerante</t>
+  </si>
+  <si>
+    <t>Ventilador Rotatorio</t>
+  </si>
+  <si>
+    <t>Compresor Solar</t>
+  </si>
+  <si>
+    <t>Par Termoeléctrico</t>
+  </si>
+  <si>
+    <t>Termostato</t>
+  </si>
+  <si>
+    <t>Termómetro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Regulador de Voltaje</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -415,6 +601,22 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial Narrow"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212121"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -439,13 +641,49 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -468,11 +706,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="40">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -870,10 +1150,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -881,7 +1161,7 @@
     <col min="1" max="1" width="16.83203125" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
     <col min="5" max="5" width="20.6640625" customWidth="1"/>
     <col min="6" max="6" width="32.83203125" customWidth="1"/>
     <col min="7" max="7" width="32.33203125" customWidth="1"/>
@@ -1046,34 +1326,57 @@
         <v>90</v>
       </c>
       <c r="H8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I8" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="30">
+      <c r="C9" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="C9" s="1" t="s">
-        <v>12</v>
+      <c r="D9" t="s">
+        <v>121</v>
       </c>
       <c r="E9" t="s">
         <v>107</v>
       </c>
       <c r="F9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G9" t="s">
+        <v>118</v>
+      </c>
+      <c r="H9" t="s">
+        <v>119</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="C10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
+        <v>114</v>
+      </c>
+      <c r="F10" t="s">
+        <v>116</v>
+      </c>
+      <c r="G10" t="s">
+        <v>117</v>
+      </c>
+      <c r="H10" t="s">
+        <v>109</v>
+      </c>
+      <c r="I10" t="s">
         <v>108</v>
       </c>
-      <c r="G9" t="s">
-        <v>109</v>
-      </c>
-      <c r="H9" t="s">
-        <v>111</v>
-      </c>
-      <c r="I9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" t="s">
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1090,10 +1393,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D7"/>
+  <dimension ref="A2:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1138,7 +1441,7 @@
         <v>92</v>
       </c>
       <c r="B4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C4" t="s">
         <v>105</v>
@@ -1188,6 +1491,264 @@
       <c r="D7" t="s">
         <v>104</v>
       </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C12" t="s">
+        <v>154</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C13" t="s">
+        <v>146</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C14" t="s">
+        <v>140</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="C15" t="s">
+        <v>156</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="19" customHeight="1">
+      <c r="A16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C16" t="s">
+        <v>144</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C17" t="s">
+        <v>153</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C18" t="s">
+        <v>155</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C19" t="s">
+        <v>151</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>121</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C20" t="s">
+        <v>152</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C21" t="s">
+        <v>150</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>121</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="C22" t="s">
+        <v>142</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>121</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="C23" t="s">
+        <v>143</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>121</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C24" t="s">
+        <v>149</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>121</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C25" t="s">
+        <v>148</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C26" t="s">
+        <v>145</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>121</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C27" t="s">
+        <v>141</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>121</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C28" t="s">
+        <v>147</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="17" customHeight="1">
+      <c r="A29" t="s">
+        <v>121</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C29" t="s">
+        <v>157</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="B30" s="10"/>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="B31" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Fix maintenance log form
</commit_message>
<xml_diff>
--- a/app/config/tables/maintenance_logs/forms/maintenance_logs/maintenance_logs.xlsx
+++ b/app/config/tables/maintenance_logs/forms/maintenance_logs/maintenance_logs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="1300" windowWidth="28360" windowHeight="19560" tabRatio="500"/>
+    <workbookView xWindow="5440" yWindow="1700" windowWidth="28360" windowHeight="19560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="149">
   <si>
     <t>clause</t>
   </si>
@@ -401,51 +401,24 @@
     <t>electric_compressor</t>
   </si>
   <si>
-    <t>thermocouple</t>
-  </si>
-  <si>
     <t xml:space="preserve">charging_cylinder </t>
   </si>
   <si>
-    <t>thermometer</t>
-  </si>
-  <si>
     <t>solar_compressor</t>
   </si>
   <si>
     <t>rotary_fan</t>
   </si>
   <si>
-    <t>leak_detector</t>
-  </si>
-  <si>
-    <t>gas_regulator</t>
-  </si>
-  <si>
-    <t>hose</t>
-  </si>
-  <si>
     <t>fridge_tag</t>
   </si>
   <si>
-    <t>refrigerant</t>
-  </si>
-  <si>
     <t>thermostat</t>
   </si>
   <si>
     <t>relay</t>
   </si>
   <si>
-    <t>burner</t>
-  </si>
-  <si>
-    <t>fuse</t>
-  </si>
-  <si>
-    <t>voltage_regulator</t>
-  </si>
-  <si>
     <t>door_gasket</t>
   </si>
   <si>
@@ -458,52 +431,22 @@
     <t>Relay</t>
   </si>
   <si>
-    <t>Refrigerant</t>
-  </si>
-  <si>
     <t>Electric Compressor</t>
   </si>
   <si>
-    <t>Thermocouple</t>
-  </si>
-  <si>
     <t>Charging Cylinder</t>
   </si>
   <si>
-    <t>Thermometer</t>
-  </si>
-  <si>
     <t>Solar Compressor</t>
   </si>
   <si>
     <t>Rotary Fan</t>
   </si>
   <si>
-    <t>Leak Detector</t>
-  </si>
-  <si>
-    <t>Gas Regulator</t>
-  </si>
-  <si>
-    <t>Hose</t>
-  </si>
-  <si>
     <t>Fridge Tag</t>
   </si>
   <si>
-    <t>Burner</t>
-  </si>
-  <si>
-    <t>Fuse</t>
-  </si>
-  <si>
     <t>Door Gasket</t>
-  </si>
-  <si>
-    <t>Voltage Regulator</t>
-  </si>
-  <si>
-    <t>Quemador</t>
   </si>
   <si>
     <t>Cilindro de carga</t>
@@ -522,41 +465,16 @@
     <t>Etiqueta Frigorífico</t>
   </si>
   <si>
-    <t>Fusible</t>
-  </si>
-  <si>
-    <t>Regulador de Gas</t>
-  </si>
-  <si>
-    <t>Manguera</t>
-  </si>
-  <si>
-    <t>Detector de Fugas</t>
-  </si>
-  <si>
     <t>Relé</t>
   </si>
   <si>
-    <t>Refrigerante</t>
-  </si>
-  <si>
     <t>Ventilador Rotatorio</t>
   </si>
   <si>
     <t>Compresor Solar</t>
   </si>
   <si>
-    <t>Par Termoeléctrico</t>
-  </si>
-  <si>
     <t>Termostato</t>
-  </si>
-  <si>
-    <t>Termómetro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Regulador de Voltaje</t>
   </si>
 </sst>
 </file>
@@ -1152,7 +1070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -1393,10 +1311,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D31"/>
+  <dimension ref="A2:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1497,13 +1415,13 @@
         <v>121</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="C12" t="s">
-        <v>154</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>158</v>
+        <v>135</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1511,13 +1429,13 @@
         <v>121</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C13" t="s">
-        <v>146</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>159</v>
+        <v>131</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1525,41 +1443,41 @@
         <v>121</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="C14" t="s">
-        <v>140</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>139</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="19" customHeight="1">
       <c r="A15" t="s">
         <v>121</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="C15" t="s">
-        <v>156</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="19" customHeight="1">
+        <v>134</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>121</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C16" t="s">
+        <v>138</v>
+      </c>
+      <c r="D16" s="12" t="s">
         <v>144</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1567,13 +1485,13 @@
         <v>121</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C17" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1581,13 +1499,13 @@
         <v>121</v>
       </c>
       <c r="B18" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C18" t="s">
         <v>137</v>
       </c>
-      <c r="C18" t="s">
-        <v>155</v>
-      </c>
       <c r="D18" s="12" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1595,13 +1513,13 @@
         <v>121</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C19" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1609,146 +1527,20 @@
         <v>121</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C20" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>121</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="C21" t="s">
-        <v>150</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>167</v>
-      </c>
+      <c r="B21" s="10"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" t="s">
-        <v>121</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="C22" t="s">
-        <v>142</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
-        <v>121</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="C23" t="s">
-        <v>143</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" t="s">
-        <v>121</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="C24" t="s">
-        <v>149</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" t="s">
-        <v>121</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="C25" t="s">
-        <v>148</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" t="s">
-        <v>121</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="C26" t="s">
-        <v>145</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" t="s">
-        <v>121</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="C27" t="s">
-        <v>141</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" t="s">
-        <v>121</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="C28" t="s">
-        <v>147</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="17" customHeight="1">
-      <c r="A29" t="s">
-        <v>121</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="C29" t="s">
-        <v>157</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="B30" s="10"/>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="B31" s="10"/>
+      <c r="B22" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Clean up maintenance form
</commit_message>
<xml_diff>
--- a/app/config/tables/maintenance_logs/forms/maintenance_logs/maintenance_logs.xlsx
+++ b/app/config/tables/maintenance_logs/forms/maintenance_logs/maintenance_logs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5440" yWindow="1700" windowWidth="28360" windowHeight="19560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="11060" yWindow="2680" windowWidth="28360" windowHeight="19560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="149">
   <si>
     <t>clause</t>
   </si>
@@ -365,9 +365,6 @@
   </si>
   <si>
     <t>upgrade</t>
-  </si>
-  <si>
-    <t>select_multiple</t>
   </si>
   <si>
     <t>addtl_spare_parts</t>
@@ -475,6 +472,9 @@
   </si>
   <si>
     <t>Termostato</t>
+  </si>
+  <si>
+    <t>select_multiple_inline</t>
   </si>
 </sst>
 </file>
@@ -1068,10 +1068,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1250,51 +1250,65 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="30">
-      <c r="C9" s="1" t="s">
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="1:10" ht="30">
+      <c r="C11" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D11" t="s">
+        <v>120</v>
+      </c>
+      <c r="E11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F11" t="s">
+        <v>114</v>
+      </c>
+      <c r="G11" t="s">
+        <v>117</v>
+      </c>
+      <c r="H11" t="s">
+        <v>118</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="C12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
         <v>113</v>
       </c>
-      <c r="D9" t="s">
-        <v>121</v>
-      </c>
-      <c r="E9" t="s">
-        <v>107</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="F12" t="s">
         <v>115</v>
       </c>
-      <c r="G9" t="s">
-        <v>118</v>
-      </c>
-      <c r="H9" t="s">
-        <v>119</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="C10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" t="s">
-        <v>114</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="G12" t="s">
         <v>116</v>
       </c>
-      <c r="G10" t="s">
-        <v>117</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="H12" t="s">
         <v>109</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
-      <c r="A11" t="s">
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1313,7 +1327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -1412,128 +1426,128 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>122</v>
-      </c>
       <c r="C13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="19" customHeight="1">
       <c r="A15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:4">

</xml_diff>

<commit_message>
Make WHO changes to maintenance_log table
</commit_message>
<xml_diff>
--- a/app/config/tables/maintenance_logs/forms/maintenance_logs/maintenance_logs.xlsx
+++ b/app/config/tables/maintenance_logs/forms/maintenance_logs/maintenance_logs.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clarice\cold-chain\cold-chain-app-designer\app\config\tables\maintenance_logs\forms\maintenance_logs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11060" yWindow="2680" windowWidth="28360" windowHeight="19560" tabRatio="500"/>
+    <workbookView xWindow="11055" yWindow="2685" windowWidth="28365" windowHeight="19560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="205">
   <si>
     <t>clause</t>
   </si>
@@ -97,12 +102,6 @@
     <t>Fecha de Servicio</t>
   </si>
   <si>
-    <t>Enter the date of service</t>
-  </si>
-  <si>
-    <t>Fecha de servicio</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
@@ -313,9 +312,6 @@
     <t>Preventative</t>
   </si>
   <si>
-    <t>Inspection</t>
-  </si>
-  <si>
     <t>Other</t>
   </si>
   <si>
@@ -325,9 +321,6 @@
     <t>preventative</t>
   </si>
   <si>
-    <t>inspection</t>
-  </si>
-  <si>
     <t>other</t>
   </si>
   <si>
@@ -337,18 +330,9 @@
     <t>Preventivo</t>
   </si>
   <si>
-    <t>Inspección</t>
-  </si>
-  <si>
     <t>Otro</t>
   </si>
   <si>
-    <t>Upgrade</t>
-  </si>
-  <si>
-    <t>Mejorar</t>
-  </si>
-  <si>
     <t>spare_parts</t>
   </si>
   <si>
@@ -362,9 +346,6 @@
   </si>
   <si>
     <t>Seleccione el tipo de mantenimiento</t>
-  </si>
-  <si>
-    <t>upgrade</t>
   </si>
   <si>
     <t>addtl_spare_parts</t>
@@ -475,13 +456,205 @@
   </si>
   <si>
     <t>select_multiple_inline</t>
+  </si>
+  <si>
+    <t>serviced_by</t>
+  </si>
+  <si>
+    <t>serviced_by_type</t>
+  </si>
+  <si>
+    <t>technician_name</t>
+  </si>
+  <si>
+    <t>Enter the date of last service</t>
+  </si>
+  <si>
+    <t>Fecha  del último servicio</t>
+  </si>
+  <si>
+    <t>next_date_serviced</t>
+  </si>
+  <si>
+    <t>Next Date Serviced</t>
+  </si>
+  <si>
+    <t>Próxima Fecha de Servicio</t>
+  </si>
+  <si>
+    <t>select_multiple</t>
+  </si>
+  <si>
+    <t>repair_types</t>
+  </si>
+  <si>
+    <t>type_of_repair</t>
+  </si>
+  <si>
+    <t>Type of Repair</t>
+  </si>
+  <si>
+    <t>preventative_maint_types</t>
+  </si>
+  <si>
+    <t>type_of_preventative_maintenance</t>
+  </si>
+  <si>
+    <t>Type of Preventative Maintenance</t>
+  </si>
+  <si>
+    <t>Serviced By</t>
+  </si>
+  <si>
+    <t>Atendido por</t>
+  </si>
+  <si>
+    <t>Who performed the service?</t>
+  </si>
+  <si>
+    <t>¿Quién realizó el servicio?</t>
+  </si>
+  <si>
+    <t>Technician Name</t>
+  </si>
+  <si>
+    <t>Nombre del técnico</t>
+  </si>
+  <si>
+    <t>Ingrese el nombre del técnico</t>
+  </si>
+  <si>
+    <t>Enter technician name</t>
+  </si>
+  <si>
+    <t>warranty_service_provider</t>
+  </si>
+  <si>
+    <t>Warranty/Service Provider</t>
+  </si>
+  <si>
+    <t>cce_technician</t>
+  </si>
+  <si>
+    <t>CCE Technician</t>
+  </si>
+  <si>
+    <t>facility_staff</t>
+  </si>
+  <si>
+    <t>Facility Staff</t>
+  </si>
+  <si>
+    <t>select_one_with_other</t>
+  </si>
+  <si>
+    <t>fridge_dryer</t>
+  </si>
+  <si>
+    <t>Fridge Dryer</t>
+  </si>
+  <si>
+    <t>electronic_control_unit</t>
+  </si>
+  <si>
+    <t>Electronic Control Unit</t>
+  </si>
+  <si>
+    <t>hinges</t>
+  </si>
+  <si>
+    <t>Hinges</t>
+  </si>
+  <si>
+    <t>need_data</t>
+  </si>
+  <si>
+    <t>Need Data</t>
+  </si>
+  <si>
+    <t>clean_solar_panels</t>
+  </si>
+  <si>
+    <t>Clean solar panels</t>
+  </si>
+  <si>
+    <t>clean_coils</t>
+  </si>
+  <si>
+    <t>Clean coils</t>
+  </si>
+  <si>
+    <t>Necesita Datos</t>
+  </si>
+  <si>
+    <t>Garantía / Proveedor de Servicios</t>
+  </si>
+  <si>
+    <t>CCE Técnico</t>
+  </si>
+  <si>
+    <t>Personal de las Facilidades</t>
+  </si>
+  <si>
+    <t>Secador de Refrigerador</t>
+  </si>
+  <si>
+    <t>Unidad de Control Electrónico</t>
+  </si>
+  <si>
+    <t>Bisagra</t>
+  </si>
+  <si>
+    <t>data('type_of_maintenance') === 'repair'</t>
+  </si>
+  <si>
+    <t>Ingrese la próxima fecha de servicio</t>
+  </si>
+  <si>
+    <t>Enter the next date serviced</t>
+  </si>
+  <si>
+    <t>Tipo de Reparación</t>
+  </si>
+  <si>
+    <t>Tipo de Mantenimiento Preventivo</t>
+  </si>
+  <si>
+    <t>Select type of repair</t>
+  </si>
+  <si>
+    <t>Seleccione tipo de reparación</t>
+  </si>
+  <si>
+    <t>Seleccione tipo de mantenimiento</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>maintenance_log_image</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>Imagen</t>
+  </si>
+  <si>
+    <t>Take a picture</t>
+  </si>
+  <si>
+    <t>Toma una foto</t>
+  </si>
+  <si>
+    <t>data('type_of_maintenance') === 'preventative'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -533,6 +706,25 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -601,7 +793,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -630,6 +822,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="40">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -743,6 +940,14 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1068,27 +1273,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="1" max="1" width="16.875" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" customWidth="1"/>
-    <col min="6" max="6" width="32.83203125" customWidth="1"/>
-    <col min="7" max="7" width="32.33203125" customWidth="1"/>
-    <col min="8" max="8" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="22.625" customWidth="1"/>
+    <col min="5" max="5" width="20.625" customWidth="1"/>
+    <col min="6" max="6" width="32.875" customWidth="1"/>
+    <col min="7" max="7" width="32.375" customWidth="1"/>
+    <col min="8" max="8" width="24.625" customWidth="1"/>
     <col min="9" max="9" width="39.5" customWidth="1"/>
     <col min="10" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1120,7 +1325,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1133,7 +1338,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1148,7 +1353,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
@@ -1174,7 +1379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1186,135 +1391,333 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:10">
-      <c r="C6" s="3" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
+      <c r="D11" s="3"/>
+      <c r="E11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H11" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="I11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
         <v>23</v>
       </c>
-      <c r="I6" t="s">
+      <c r="F13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="C7" t="s">
+      <c r="G13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" t="s">
+        <v>86</v>
+      </c>
+      <c r="F14" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H14" t="s">
+        <v>103</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>190</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D16" t="s">
+        <v>150</v>
+      </c>
+      <c r="E16" t="s">
+        <v>151</v>
+      </c>
+      <c r="F16" t="s">
+        <v>152</v>
+      </c>
+      <c r="G16" t="s">
+        <v>193</v>
+      </c>
+      <c r="H16" t="s">
+        <v>195</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>204</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D19" t="s">
+        <v>153</v>
+      </c>
+      <c r="E19" t="s">
+        <v>154</v>
+      </c>
+      <c r="F19" t="s">
+        <v>155</v>
+      </c>
+      <c r="G19" t="s">
+        <v>194</v>
+      </c>
+      <c r="H19" t="s">
+        <v>103</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="I21" s="9"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="I22" s="9"/>
+    </row>
+    <row r="23" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C23" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D23" t="s">
+        <v>112</v>
+      </c>
+      <c r="E23" t="s">
+        <v>100</v>
+      </c>
+      <c r="F23" t="s">
+        <v>106</v>
+      </c>
+      <c r="G23" t="s">
+        <v>109</v>
+      </c>
+      <c r="H23" t="s">
+        <v>110</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="E24" t="s">
+        <v>105</v>
+      </c>
+      <c r="F24" t="s">
+        <v>107</v>
+      </c>
+      <c r="G24" t="s">
+        <v>108</v>
+      </c>
+      <c r="H24" t="s">
+        <v>102</v>
+      </c>
+      <c r="I24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>28</v>
-      </c>
-      <c r="I7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="C8" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D8" t="s">
-        <v>92</v>
-      </c>
-      <c r="E8" t="s">
-        <v>88</v>
-      </c>
-      <c r="F8" t="s">
-        <v>89</v>
-      </c>
-      <c r="G8" t="s">
-        <v>90</v>
-      </c>
-      <c r="H8" t="s">
-        <v>110</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="I9" s="9"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="I10" s="9"/>
-    </row>
-    <row r="11" spans="1:10" ht="30">
-      <c r="C11" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D11" t="s">
-        <v>120</v>
-      </c>
-      <c r="E11" t="s">
-        <v>107</v>
-      </c>
-      <c r="F11" t="s">
-        <v>114</v>
-      </c>
-      <c r="G11" t="s">
-        <v>117</v>
-      </c>
-      <c r="H11" t="s">
-        <v>118</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="C12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" t="s">
-        <v>113</v>
-      </c>
-      <c r="F12" t="s">
-        <v>115</v>
-      </c>
-      <c r="G12" t="s">
-        <v>116</v>
-      </c>
-      <c r="H12" t="s">
-        <v>109</v>
-      </c>
-      <c r="I12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1325,236 +1728,336 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D22"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" customWidth="1"/>
+    <col min="1" max="1" width="23.125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.375" customWidth="1"/>
+    <col min="4" max="4" width="20.375" customWidth="1"/>
     <col min="5" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="20" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    <row r="1" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" t="s">
+        <v>91</v>
+      </c>
       <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" t="s">
         <v>92</v>
       </c>
-      <c r="B3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" t="s">
         <v>93</v>
       </c>
-      <c r="D3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6" t="s">
+        <v>165</v>
+      </c>
+      <c r="D6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C8" t="s">
+        <v>169</v>
+      </c>
+      <c r="D8" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>112</v>
       </c>
-      <c r="C4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>92</v>
-      </c>
-      <c r="B7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="B10" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" t="s">
+        <v>122</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C12" t="s">
+        <v>130</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" t="s">
+        <v>125</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="C15" t="s">
+        <v>124</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C16" t="s">
+        <v>128</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" t="s">
+        <v>127</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" t="s">
         <v>123</v>
       </c>
-      <c r="C12" t="s">
-        <v>134</v>
-      </c>
-      <c r="D12" s="12" t="s">
+      <c r="D18" s="12" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>120</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="C13" t="s">
-        <v>130</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>120</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="C14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="19" customHeight="1">
-      <c r="A15" t="s">
-        <v>120</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="C15" t="s">
-        <v>133</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>120</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="C16" t="s">
-        <v>137</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>120</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="C17" t="s">
-        <v>132</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>120</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="C18" t="s">
-        <v>136</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>120</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>124</v>
+        <v>112</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>171</v>
       </c>
       <c r="C19" t="s">
-        <v>135</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>172</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>120</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>127</v>
+        <v>112</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>173</v>
       </c>
       <c r="C20" t="s">
-        <v>131</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="B21" s="10"/>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="B22" s="10"/>
+        <v>174</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="C21" t="s">
+        <v>176</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>150</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="C23" t="s">
+        <v>178</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>153</v>
+      </c>
+      <c r="B25" t="s">
+        <v>179</v>
+      </c>
+      <c r="C25" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>153</v>
+      </c>
+      <c r="B26" t="s">
+        <v>181</v>
+      </c>
+      <c r="C26" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>153</v>
+      </c>
+      <c r="B27" t="s">
+        <v>177</v>
+      </c>
+      <c r="C27" t="s">
+        <v>178</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>183</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1575,69 +2078,69 @@
       <selection activeCell="A3" activeCellId="1" sqref="B5 A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.375" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="29.83203125" customWidth="1"/>
+    <col min="5" max="5" width="29.875" customWidth="1"/>
     <col min="6" max="6" width="35" customWidth="1"/>
-    <col min="7" max="7" width="47.1640625" customWidth="1"/>
-    <col min="8" max="8" width="38.83203125" customWidth="1"/>
+    <col min="7" max="7" width="47.125" customWidth="1"/>
+    <col min="8" max="8" width="38.875" customWidth="1"/>
     <col min="9" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="5" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="B2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
         <v>41</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
         <v>42</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>43</v>
       </c>
-      <c r="D2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="G2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="H2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1659,22 +2162,22 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="8.5" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" customWidth="1"/>
-    <col min="5" max="5" width="29.1640625" customWidth="1"/>
+    <col min="3" max="3" width="19.875" customWidth="1"/>
+    <col min="4" max="4" width="17.125" customWidth="1"/>
+    <col min="5" max="5" width="29.125" customWidth="1"/>
     <col min="6" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -1683,75 +2186,75 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>49</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>51</v>
       </c>
-      <c r="B2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
+      <c r="C4" t="s">
         <v>52</v>
       </c>
-      <c r="B3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
+      <c r="D4" t="s">
         <v>53</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="D4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="6" t="s">
-        <v>56</v>
       </c>
       <c r="B5" s="6">
         <v>20170804</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" t="s">
         <v>58</v>
       </c>
-      <c r="E7" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>59</v>
       </c>
-      <c r="F7" t="s">
+      <c r="E8" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
+      <c r="F8" t="s">
         <v>61</v>
-      </c>
-      <c r="E8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F8" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1773,149 +2276,149 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.5" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" customWidth="1"/>
+    <col min="3" max="3" width="22.625" customWidth="1"/>
+    <col min="4" max="4" width="20.125" customWidth="1"/>
     <col min="5" max="5" width="17.5" customWidth="1"/>
     <col min="6" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
         <v>64</v>
-      </c>
-      <c r="B1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" t="s">
-        <v>66</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>67</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>69</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="E5" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="3" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>80</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update maintenance log form
</commit_message>
<xml_diff>
--- a/app/config/tables/maintenance_logs/forms/maintenance_logs/maintenance_logs.xlsx
+++ b/app/config/tables/maintenance_logs/forms/maintenance_logs/maintenance_logs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="482">
   <si>
     <t>clause</t>
   </si>
@@ -1404,45 +1404,6 @@
     <t>Ingrese comentarios</t>
   </si>
   <si>
-    <t>Select Electrical and Control System spare parts replaced/used</t>
-  </si>
-  <si>
-    <t>Select Hardware spare parts replaced/used</t>
-  </si>
-  <si>
-    <t>Select Monitoring spare parts replaced/used</t>
-  </si>
-  <si>
-    <t>Select Power spare parts replaced/used</t>
-  </si>
-  <si>
-    <t>Select Refrigeration System spare parts replaced/used</t>
-  </si>
-  <si>
-    <t>Select Solar spare parts replaced/used</t>
-  </si>
-  <si>
-    <t>Other spare parts replaced/used</t>
-  </si>
-  <si>
-    <t>Seleccione las piezas de repuesto del sistema eléctrico y de control reemplazadas/usadas</t>
-  </si>
-  <si>
-    <t>Seleccione Monitoreo de repuestos reemplazados/usados</t>
-  </si>
-  <si>
-    <t>Seleccionar repuestos de potencia reemplazados/usados</t>
-  </si>
-  <si>
-    <t>Seleccione piezas de repuesto de hardware reemplazadas/usadas</t>
-  </si>
-  <si>
-    <t>Seleccione los repuestos del sistema de refrigeración reemplazados/usados</t>
-  </si>
-  <si>
-    <t>Seleccionar repuestos solares reemplazados/usados</t>
-  </si>
-  <si>
     <t>Otras piezas de repuesto reemplazadas/usadas</t>
   </si>
   <si>
@@ -1455,9 +1416,6 @@
     <t>preventative_comments</t>
   </si>
   <si>
-    <t>selected(data('type_of_maintenance'),  'repair')</t>
-  </si>
-  <si>
     <t>selected(data('type_of_maintenance'), 'preventative')</t>
   </si>
   <si>
@@ -1465,6 +1423,54 @@
   </si>
   <si>
     <t>Seleccione tipo de mantenimiento preventivo</t>
+  </si>
+  <si>
+    <t>Select &lt;strong&gt;Electrical and Control System&lt;/strong&gt; parts replaced/used</t>
+  </si>
+  <si>
+    <t>Select &lt;strong&gt;Hardware&lt;/strong&gt; parts replaced/used</t>
+  </si>
+  <si>
+    <t>Select &lt;strong&gt;Monitoring&lt;/strong&gt; parts replaced/used</t>
+  </si>
+  <si>
+    <t>Select &lt;strong&gt;Power&lt;/strong&gt; parts replaced/used</t>
+  </si>
+  <si>
+    <t>Select &lt;strong&gt;Refrigeration System&lt;/strong&gt; parts replaced/used</t>
+  </si>
+  <si>
+    <t>Select &lt;strong&gt;Solar&lt;/strong&gt; parts replaced/used</t>
+  </si>
+  <si>
+    <t>Other parts replaced/used</t>
+  </si>
+  <si>
+    <t>Seleccione las piezas del &lt;strong&gt;sistema eléctrico y de control&lt;/strong&gt; reemplazadas/usadas</t>
+  </si>
+  <si>
+    <t>Seleccione piezas de &lt;strong&gt;hardware&lt;/strong&gt; reemplazadas/usadas</t>
+  </si>
+  <si>
+    <t>Seleccione las piezas de &lt;strong&gt;Monitoreo&lt;/strong&gt; reemplazados/usados</t>
+  </si>
+  <si>
+    <t>Seleccione las piezas del &lt;strong&gt;sistema de refrigeración&lt;/strong&gt; reemplazados/usados</t>
+  </si>
+  <si>
+    <t>Seleccione las piezas de &lt;strong&gt;potencia&lt;/strong&gt; reemplazados/usados</t>
+  </si>
+  <si>
+    <t>Seleccione las piezas de &lt;strong&gt;solares&lt;/strong&gt; reemplazados/usados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end if </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> selected(data('type_of_maintenance'),  'repair')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected(data('type_of_maintenance'),  'repair') || selected(data('type_of_maintenance'), 'other') </t>
   </si>
 </sst>
 </file>
@@ -2201,10 +2207,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L39"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2213,7 +2219,7 @@
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="26.08203125" customWidth="1"/>
-    <col min="5" max="5" width="20.58203125" customWidth="1"/>
+    <col min="5" max="5" width="25.08203125" customWidth="1"/>
     <col min="6" max="6" width="32.83203125" customWidth="1"/>
     <col min="7" max="8" width="32.33203125" customWidth="1"/>
     <col min="9" max="9" width="24.58203125" customWidth="1"/>
@@ -2431,120 +2437,120 @@
       <c r="J9" s="1"/>
       <c r="K9" s="22"/>
     </row>
-    <row r="10" spans="1:12" s="30" customFormat="1" ht="31" x14ac:dyDescent="0.35">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="22"/>
+    </row>
+    <row r="11" spans="1:12" s="30" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="31" t="s">
+        <v>355</v>
+      </c>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>395</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31" t="s">
+        <v>396</v>
+      </c>
+      <c r="J11" s="30" t="s">
+        <v>397</v>
+      </c>
+      <c r="K11" s="32" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="22" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C13" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" t="s">
+        <v>85</v>
+      </c>
+      <c r="G13" t="s">
+        <v>86</v>
+      </c>
+      <c r="I13" t="s">
+        <v>97</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="K13" s="22" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="30" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A14" s="32"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32" t="s">
         <v>168</v>
       </c>
-      <c r="D10" s="33"/>
-      <c r="E10" s="32" t="s">
+      <c r="D14" s="33"/>
+      <c r="E14" s="32" t="s">
         <v>169</v>
       </c>
-      <c r="F10" s="32" t="s">
+      <c r="F14" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="G10" s="32" t="s">
+      <c r="G14" s="32" t="s">
         <v>171</v>
       </c>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32" t="s">
+      <c r="H14" s="32"/>
+      <c r="I14" s="32" t="s">
         <v>401</v>
       </c>
-      <c r="J10" s="32" t="s">
+      <c r="J14" s="32" t="s">
         <v>172</v>
       </c>
-      <c r="K10" s="32" t="s">
+      <c r="K14" s="32" t="s">
         <v>378</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="22"/>
-    </row>
-    <row r="12" spans="1:12" s="30" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="31" t="s">
-        <v>355</v>
-      </c>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="31" t="s">
-        <v>395</v>
-      </c>
-      <c r="G12" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31" t="s">
-        <v>396</v>
-      </c>
-      <c r="J12" s="30" t="s">
-        <v>397</v>
-      </c>
-      <c r="K12" s="32" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="31" x14ac:dyDescent="0.35">
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J13" t="s">
-        <v>25</v>
-      </c>
-      <c r="K13" s="22" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="C14" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D14" t="s">
-        <v>87</v>
-      </c>
-      <c r="E14" t="s">
-        <v>84</v>
-      </c>
-      <c r="F14" t="s">
-        <v>85</v>
-      </c>
-      <c r="G14" t="s">
-        <v>86</v>
-      </c>
-      <c r="I14" t="s">
-        <v>97</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="K14" s="22" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="15" spans="1:12" s="28" customFormat="1" x14ac:dyDescent="0.35">
@@ -2592,7 +2598,7 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="C18" s="1"/>
       <c r="J18" s="9"/>
@@ -2698,7 +2704,7 @@
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>477</v>
+        <v>463</v>
       </c>
       <c r="C25" s="1"/>
       <c r="J25" s="9"/>
@@ -2721,10 +2727,10 @@
         <v>165</v>
       </c>
       <c r="I26" s="30" t="s">
-        <v>478</v>
+        <v>464</v>
       </c>
       <c r="J26" s="34" t="s">
-        <v>479</v>
+        <v>465</v>
       </c>
       <c r="K26" s="34" t="s">
         <v>380</v>
@@ -2735,7 +2741,7 @@
         <v>402</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>475</v>
+        <v>462</v>
       </c>
       <c r="F27" s="30" t="s">
         <v>403</v>
@@ -2764,82 +2770,68 @@
       <c r="J29" s="9"/>
       <c r="K29" s="20"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>10</v>
+    <row r="30" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="28" t="s">
+        <v>481</v>
       </c>
       <c r="C30" s="1"/>
       <c r="J30" s="9"/>
-      <c r="K30" s="20"/>
-    </row>
-    <row r="31" spans="1:11" s="30" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C31" s="32" t="s">
-        <v>339</v>
-      </c>
-      <c r="D31" s="30" t="s">
-        <v>340</v>
-      </c>
-      <c r="E31" s="30" t="s">
-        <v>345</v>
-      </c>
-      <c r="F31" s="30" t="s">
-        <v>179</v>
-      </c>
-      <c r="G31" s="30" t="s">
-        <v>184</v>
-      </c>
-      <c r="I31" s="30" t="s">
-        <v>459</v>
-      </c>
-      <c r="J31" s="34" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="20"/>
+    </row>
+    <row r="32" spans="1:11" s="30" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C32" s="32" t="s">
         <v>339</v>
       </c>
       <c r="D32" s="30" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F32" s="30" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G32" s="30" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="I32" s="30" t="s">
-        <v>460</v>
+        <v>466</v>
       </c>
       <c r="J32" s="34" t="s">
-        <v>469</v>
-      </c>
-      <c r="K32" s="34"/>
+        <v>473</v>
+      </c>
     </row>
     <row r="33" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C33" s="32" t="s">
         <v>339</v>
       </c>
       <c r="D33" s="30" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F33" s="30" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G33" s="30" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="I33" s="30" t="s">
-        <v>461</v>
+        <v>467</v>
       </c>
       <c r="J33" s="34" t="s">
-        <v>467</v>
+        <v>474</v>
       </c>
       <c r="K33" s="34"/>
     </row>
@@ -2848,114 +2840,143 @@
         <v>339</v>
       </c>
       <c r="D34" s="30" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F34" s="30" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G34" s="30" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I34" s="30" t="s">
-        <v>462</v>
+        <v>468</v>
       </c>
       <c r="J34" s="34" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="K34" s="34"/>
     </row>
-    <row r="35" spans="1:11" s="30" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C35" s="32" t="s">
         <v>339</v>
       </c>
       <c r="D35" s="30" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F35" s="30" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="G35" s="30" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I35" s="30" t="s">
-        <v>463</v>
+        <v>469</v>
       </c>
       <c r="J35" s="34" t="s">
-        <v>470</v>
+        <v>477</v>
       </c>
       <c r="K35" s="34"/>
     </row>
-    <row r="36" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" s="30" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="C36" s="32" t="s">
         <v>339</v>
       </c>
       <c r="D36" s="30" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F36" s="30" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="G36" s="30" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="I36" s="30" t="s">
-        <v>464</v>
+        <v>470</v>
       </c>
       <c r="J36" s="34" t="s">
-        <v>471</v>
+        <v>476</v>
       </c>
       <c r="K36" s="34"/>
     </row>
     <row r="37" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C37" s="32" t="s">
+        <v>339</v>
+      </c>
+      <c r="D37" s="30" t="s">
+        <v>344</v>
+      </c>
+      <c r="E37" s="30" t="s">
+        <v>351</v>
+      </c>
+      <c r="F37" s="30" t="s">
+        <v>183</v>
+      </c>
+      <c r="G37" s="30" t="s">
+        <v>183</v>
+      </c>
+      <c r="I37" s="30" t="s">
+        <v>471</v>
+      </c>
+      <c r="J37" s="34" t="s">
+        <v>478</v>
+      </c>
+      <c r="K37" s="34"/>
+    </row>
+    <row r="38" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C38" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E37" s="30" t="s">
+      <c r="E38" s="30" t="s">
         <v>455</v>
       </c>
-      <c r="F37" s="30" t="s">
+      <c r="F38" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="G37" s="30" t="s">
+      <c r="G38" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="I37" s="30" t="s">
-        <v>465</v>
-      </c>
-      <c r="J37" s="30" t="s">
+      <c r="I38" s="30" t="s">
         <v>472</v>
       </c>
-      <c r="K37" s="34"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+      <c r="J38" s="30" t="s">
+        <v>459</v>
+      </c>
+      <c r="K38" s="34"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C39" s="32" t="s">
+    <row r="40" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C40" s="32" t="s">
         <v>410</v>
       </c>
-      <c r="F39" s="30" t="s">
-        <v>473</v>
-      </c>
-      <c r="G39" s="30" t="s">
-        <v>474</v>
-      </c>
-      <c r="I39" s="30" t="s">
+      <c r="F40" s="30" t="s">
+        <v>460</v>
+      </c>
+      <c r="G40" s="30" t="s">
+        <v>461</v>
+      </c>
+      <c r="I40" s="30" t="s">
         <v>437</v>
       </c>
-      <c r="J39" s="30" t="s">
+      <c r="J40" s="30" t="s">
         <v>456</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>479</v>
       </c>
     </row>
   </sheetData>

</xml_diff>